<commit_message>
remove 1 row in excel and added a comment
</commit_message>
<xml_diff>
--- a/data/TC001.xlsx
+++ b/data/TC001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15300" windowHeight="4056"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="15300" windowHeight="4050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>UserName</t>
   </si>
@@ -28,12 +28,6 @@
   </si>
   <si>
     <t>crmsfa</t>
-  </si>
-  <si>
-    <t>DemoCSR</t>
-  </si>
-  <si>
-    <t>Demo B2B CSR</t>
   </si>
   <si>
     <t>Verify</t>
@@ -50,7 +44,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tunga"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -394,16 +388,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="22.5"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -414,7 +408,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -425,17 +419,6 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -451,7 +434,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="22.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -463,7 +446,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="22.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>